<commit_message>
order ampli1 lib primers
</commit_message>
<xml_diff>
--- a/notebooks_terra/ampli_lib_primer_fixed.xlsx
+++ b/notebooks_terra/ampli_lib_primer_fixed.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taol9/gitsss/yo/notebooks_terra/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F961A8-5777-624A-BA0A-6CA47E0B6BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="820" yWindow="460" windowWidth="28340" windowHeight="20980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -1183,8 +1189,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1247,6 +1253,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1293,7 +1307,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1325,9 +1339,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1359,6 +1391,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1534,14 +1584,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10:E17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="77.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1555,7 +1613,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1572,7 +1630,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1589,7 +1647,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1606,7 +1664,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1623,7 +1681,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1640,7 +1698,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1657,7 +1715,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1674,7 +1732,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1691,7 +1749,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1708,7 +1766,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1725,7 +1783,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1742,7 +1800,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1759,7 +1817,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1776,7 +1834,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1793,7 +1851,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1810,7 +1868,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1827,7 +1885,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1844,7 +1902,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1861,7 +1919,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1878,7 +1936,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1895,7 +1953,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1912,7 +1970,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1929,7 +1987,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1946,7 +2004,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1963,7 +2021,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1980,7 +2038,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1997,7 +2055,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2014,7 +2072,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2031,7 +2089,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2048,7 +2106,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2065,7 +2123,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2082,7 +2140,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2099,7 +2157,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2116,7 +2174,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2133,7 +2191,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -2150,7 +2208,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -2167,7 +2225,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -2184,7 +2242,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -2201,7 +2259,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2218,7 +2276,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -2235,7 +2293,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -2252,7 +2310,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2269,7 +2327,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -2286,7 +2344,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -2303,7 +2361,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -2320,7 +2378,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -2337,7 +2395,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -2354,7 +2412,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -2371,7 +2429,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -2388,7 +2446,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -2405,7 +2463,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -2422,7 +2480,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -2439,7 +2497,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -2456,7 +2514,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -2473,7 +2531,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -2490,7 +2548,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -2507,7 +2565,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2524,7 +2582,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -2541,7 +2599,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2558,7 +2616,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -2575,7 +2633,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -2592,7 +2650,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -2609,7 +2667,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -2626,7 +2684,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -2643,7 +2701,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -2660,7 +2718,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -2677,7 +2735,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -2694,7 +2752,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -2711,7 +2769,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -2728,7 +2786,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -2745,7 +2803,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -2762,7 +2820,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -2779,7 +2837,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -2796,7 +2854,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -2813,7 +2871,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -2830,7 +2888,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -2847,7 +2905,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -2864,7 +2922,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -2881,7 +2939,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -2898,7 +2956,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -2915,7 +2973,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -2932,7 +2990,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -2949,7 +3007,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -2966,7 +3024,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -2983,7 +3041,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -3000,7 +3058,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -3017,7 +3075,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -3034,7 +3092,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -3051,7 +3109,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -3068,7 +3126,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -3085,7 +3143,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -3102,7 +3160,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -3119,7 +3177,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -3136,7 +3194,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -3153,7 +3211,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -3170,7 +3228,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>95</v>
       </c>

</xml_diff>